<commit_message>
update timesheet: please use .xlsx instead of .xls, as my computer can't save to .xls. sorry"
</commit_message>
<xml_diff>
--- a/timeSheet.xlsx
+++ b/timeSheet.xlsx
@@ -1289,9 +1289,15 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>42670.479166666664</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42670.5</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>

</xml_diff>

<commit_message>
Removed duplicate timeSheet and updated proposal
Updated project proposal and group resume.
</commit_message>
<xml_diff>
--- a/timeSheet.xlsx
+++ b/timeSheet.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView windowWidth="23895" windowHeight="10380"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
   <si>
     <t>To insert the current date and time, press Ctrl+; (semi-colon), then press Space, and then press Ctrl+Shift+; (semi-colon).</t>
   </si>
@@ -40,32 +43,178 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,11 +224,197 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor auto="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -102,63 +437,399 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Comma[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Currency[0]" xfId="6" builtinId="7"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00AAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -357,8 +1028,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
@@ -378,8 +1047,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -408,8 +1076,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -434,8 +1101,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -460,8 +1126,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -486,8 +1151,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -512,8 +1176,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -538,8 +1201,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -564,8 +1226,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -590,8 +1251,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -616,8 +1276,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -630,9 +1289,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -646,8 +1311,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -667,8 +1330,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -693,8 +1355,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -719,8 +1380,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -745,8 +1405,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -771,8 +1430,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -797,8 +1455,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -823,8 +1480,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,8 +1505,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,8 +1530,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,8 +1555,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,9 +1568,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -928,8 +1587,6 @@
           <a:noFill/>
           <a:miter lim="400000"/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
@@ -949,8 +1606,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,8 +1635,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,8 +1660,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,8 +1685,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1057,8 +1710,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1083,8 +1735,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1109,8 +1760,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1135,8 +1785,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1161,8 +1810,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1187,8 +1835,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,82 +1848,90 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="1" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5047619047619" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5047619047619" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1714285714286" style="1" customWidth="1"/>
+    <col min="4" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="53" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" ht="53" customHeight="1" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5">
-        <v>42666.415972222225</v>
+        <v>42666.4159722222</v>
       </c>
       <c r="C3" s="5">
-        <v>42666.509722222225</v>
+        <v>42666.5097222222</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>42666.927083333336</v>
+        <v>42666.9270833333</v>
       </c>
       <c r="C4" s="5">
-        <v>42669.958333333336</v>
+        <v>42669.9583333333</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5">
@@ -1285,47 +1940,53 @@
       <c r="C5" s="5">
         <v>42669.90625</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>42670.5138888889</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42670.5263888889</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="0.979861111111111" bottom="0.979861111111111" header="0.509722222222222" footer="0.509722222222222"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1333,94 +1994,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="6" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="6" customWidth="1"/>
+    <col min="1" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722222222222" footer="0.509722222222222"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1428,94 +2087,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="7" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="7" customWidth="1"/>
+    <col min="1" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722222222222" footer="0.509722222222222"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Finished Neural Network Implementation
See title
</commit_message>
<xml_diff>
--- a/timeSheet.xlsx
+++ b/timeSheet.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView windowWidth="28695" windowHeight="13080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
   <si>
     <t>To insert the current date and time, press Ctrl+; (semi-colon), then press Space, and then press Ctrl+Shift+; (semi-colon).</t>
   </si>
@@ -40,32 +43,178 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,11 +224,197 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor auto="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -102,63 +437,402 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Comma[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Currency[0]" xfId="6" builtinId="7"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00AAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -357,8 +1031,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
@@ -378,8 +1050,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -408,8 +1079,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -434,8 +1104,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -460,8 +1129,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -486,8 +1154,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -512,8 +1179,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -538,8 +1204,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -564,8 +1229,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -590,8 +1254,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -616,8 +1279,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -630,9 +1292,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -646,8 +1314,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -667,8 +1333,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -693,8 +1358,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -719,8 +1383,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -745,8 +1408,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -771,8 +1433,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -797,8 +1458,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -823,8 +1483,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,8 +1508,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,8 +1533,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,8 +1558,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,9 +1571,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -928,8 +1590,6 @@
           <a:noFill/>
           <a:miter lim="400000"/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
@@ -949,8 +1609,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,8 +1638,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,8 +1663,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,8 +1688,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1057,8 +1713,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1083,8 +1738,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1109,8 +1763,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1135,8 +1788,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1161,8 +1813,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1187,8 +1838,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,56 +1851,64 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="1" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5047619047619" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5047619047619" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1714285714286" style="1" customWidth="1"/>
+    <col min="4" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="53" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" ht="53" customHeight="1" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5">
@@ -1259,11 +1917,11 @@
       <c r="C3" s="5">
         <v>42666.5097222222</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5">
@@ -1272,11 +1930,11 @@
       <c r="C4" s="5">
         <v>42669.9583333333</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5">
@@ -1285,11 +1943,11 @@
       <c r="C5" s="5">
         <v>42669.90625</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5">
@@ -1298,11 +1956,11 @@
       <c r="C6" s="5">
         <v>42670.5263888889</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5">
@@ -1311,11 +1969,11 @@
       <c r="C7" s="5">
         <v>42676.625</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="4">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5">
@@ -1324,11 +1982,11 @@
       <c r="C8" s="5">
         <v>42676.625</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="4">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5">
@@ -1337,11 +1995,11 @@
       <c r="C9" s="5">
         <v>42689</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="4">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5">
@@ -1350,38 +2008,49 @@
       <c r="C10" s="5">
         <v>42689</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" t="s" s="4">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5">
-        <v>42689.638888888891</v>
+        <v>42689.6388888889</v>
       </c>
       <c r="C11" s="5">
-        <v>42689.757638888892</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" t="s" s="4">
+        <v>42689.7576388889</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="5">
-        <v>42689.638888888891</v>
+        <v>42689.6388888889</v>
       </c>
       <c r="C12" s="5">
-        <v>42689.757638888892</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+        <v>42689.7576388889</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6">
+        <v>42690.9847222222</v>
+      </c>
+      <c r="C13" s="6">
+        <v>42691.15</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.979861" bottom="0.979861" header="0.509722" footer="0.509722"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="0.979166666666667" bottom="0.979166666666667" header="0.509027777777778" footer="0.509027777777778"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1389,94 +2058,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="6" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="6" customWidth="1"/>
+    <col min="1" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722" footer="0.509722"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1484,94 +2151,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="7" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="7" customWidth="1"/>
+    <col min="1" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722" footer="0.509722"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated timesheet nov16 and 17
</commit_message>
<xml_diff>
--- a/timeSheet.xlsx
+++ b/timeSheet.xlsx
@@ -1213,7 +1213,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1378,6 +1378,45 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
+    </row>
+    <row r="13" ht="13.65" customHeight="1">
+      <c r="A13" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5">
+        <v>42690.791666666664</v>
+      </c>
+      <c r="C13" s="5">
+        <v>42690.875</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" ht="13.65" customHeight="1">
+      <c r="A14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5">
+        <v>42690.791666666664</v>
+      </c>
+      <c r="C14" s="5">
+        <v>42690.875</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" ht="13.65" customHeight="1">
+      <c r="A15" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5">
+        <v>42691.458333333336</v>
+      </c>
+      <c r="C15" s="5">
+        <v>42691.483333333330</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.979861" bottom="0.979861" header="0.509722" footer="0.509722"/>

</xml_diff>

<commit_message>
updating timesheet: problem set
</commit_message>
<xml_diff>
--- a/timeSheet.xlsx
+++ b/timeSheet.xlsx
@@ -79,7 +79,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -102,13 +102,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -125,6 +212,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1213,7 +1336,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1358,10 +1481,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="5">
-        <v>42689.638888888891</v>
+        <v>42689.6388888889</v>
       </c>
       <c r="C11" s="5">
-        <v>42689.757638888892</v>
+        <v>42689.7576388889</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1371,55 +1494,81 @@
         <v>5</v>
       </c>
       <c r="B12" s="5">
-        <v>42689.638888888891</v>
+        <v>42689.6388888889</v>
       </c>
       <c r="C12" s="5">
-        <v>42689.757638888892</v>
+        <v>42689.7576388889</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" t="s" s="4">
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" t="s" s="6">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7">
+        <v>42690.9847222222</v>
+      </c>
+      <c r="C13" s="7">
+        <v>42691.15</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="B14" s="11">
+        <v>42691.4576388889</v>
+      </c>
+      <c r="C14" s="11">
+        <v>42691.5381944444</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11">
+        <v>42705.0263888889</v>
+      </c>
+      <c r="C15" s="11">
+        <v>42705.2583333333</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" t="s" s="10">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11">
+        <v>42717.8125</v>
+      </c>
+      <c r="C16" s="11">
+        <v>42717.972222222219</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" t="s" s="14">
         <v>6</v>
       </c>
-      <c r="B13" s="5">
-        <v>42690.791666666664</v>
-      </c>
-      <c r="C13" s="5">
-        <v>42690.875</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="B14" s="5">
-        <v>42690.791666666664</v>
-      </c>
-      <c r="C14" s="5">
-        <v>42690.875</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="B15" s="5">
-        <v>42691.458333333336</v>
-      </c>
-      <c r="C15" s="5">
-        <v>42691.483333333330</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="B17" s="15">
+        <v>42717.8125</v>
+      </c>
+      <c r="C17" s="15">
+        <v>42717.972222222219</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.979861" bottom="0.979861" header="0.509722" footer="0.509722"/>
+  <pageMargins left="0.75" right="0.75" top="0.979167" bottom="0.979167" header="0.509028" footer="0.509028"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -1435,12 +1584,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="6" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.17188" style="18" customWidth="1"/>
+    <col min="2" max="2" width="9.17188" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.17188" style="18" customWidth="1"/>
+    <col min="4" max="4" width="9.17188" style="18" customWidth="1"/>
+    <col min="5" max="5" width="9.17188" style="18" customWidth="1"/>
+    <col min="6" max="256" width="9.17188" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1514,7 +1663,7 @@
       <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722" footer="0.509722"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509028" footer="0.509028"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -1530,12 +1679,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="7" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.17188" style="19" customWidth="1"/>
+    <col min="2" max="2" width="9.17188" style="19" customWidth="1"/>
+    <col min="3" max="3" width="9.17188" style="19" customWidth="1"/>
+    <col min="4" max="4" width="9.17188" style="19" customWidth="1"/>
+    <col min="5" max="5" width="9.17188" style="19" customWidth="1"/>
+    <col min="6" max="256" width="9.17188" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1609,7 +1758,7 @@
       <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722" footer="0.509722"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509028" footer="0.509028"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>

<commit_message>
Final fixes + User manual
Final bug fixes and user's manual write up. Published via andrew
publish.
</commit_message>
<xml_diff>
--- a/timeSheet.xlsx
+++ b/timeSheet.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView windowWidth="28695" windowHeight="13080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
   <si>
     <t>To insert the current date and time, press Ctrl+; (semi-colon), then press Space, and then press Ctrl+Shift+; (semi-colon).</t>
   </si>
@@ -40,32 +43,178 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,11 +224,197 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor auto="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -144,13 +479,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -189,99 +517,438 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Comma[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Currency[0]" xfId="6" builtinId="7"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00AAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -480,8 +1147,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
@@ -501,8 +1166,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -531,8 +1195,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -557,8 +1220,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -583,8 +1245,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -609,8 +1270,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -635,8 +1295,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -661,8 +1320,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -687,8 +1345,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -713,8 +1370,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -739,8 +1395,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -753,9 +1408,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -769,8 +1430,6 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -790,8 +1449,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -816,8 +1474,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -842,8 +1499,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -868,8 +1524,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -894,8 +1549,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,8 +1574,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -946,8 +1599,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,8 +1624,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -998,8 +1649,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1024,8 +1674,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,9 +1687,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1051,8 +1706,6 @@
           <a:noFill/>
           <a:miter lim="400000"/>
         </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
@@ -1072,8 +1725,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1102,8 +1754,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1128,8 +1779,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1154,8 +1804,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1180,8 +1829,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1206,8 +1854,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1232,8 +1879,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1258,8 +1904,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1284,8 +1929,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1310,8 +1954,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1324,56 +1967,64 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="1" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5047619047619" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5047619047619" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1714285714286" style="1" customWidth="1"/>
+    <col min="4" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="53" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" ht="53" customHeight="1" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5">
@@ -1382,11 +2033,11 @@
       <c r="C3" s="5">
         <v>42666.5097222222</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5">
@@ -1395,11 +2046,11 @@
       <c r="C4" s="5">
         <v>42669.9583333333</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5">
@@ -1408,11 +2059,11 @@
       <c r="C5" s="5">
         <v>42669.90625</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5">
@@ -1421,11 +2072,11 @@
       <c r="C6" s="5">
         <v>42670.5263888889</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5">
@@ -1434,11 +2085,11 @@
       <c r="C7" s="5">
         <v>42676.625</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="4">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5">
@@ -1447,11 +2098,11 @@
       <c r="C8" s="5">
         <v>42676.625</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="4">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5">
@@ -1460,11 +2111,11 @@
       <c r="C9" s="5">
         <v>42689</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="4">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5">
@@ -1473,11 +2124,11 @@
       <c r="C10" s="5">
         <v>42689</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" t="s" s="4">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5">
@@ -1486,11 +2137,11 @@
       <c r="C11" s="5">
         <v>42689.7576388889</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" t="s" s="4">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="5">
@@ -1499,11 +2150,11 @@
       <c r="C12" s="5">
         <v>42689.7576388889</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="6">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:5">
+      <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="7">
@@ -1515,8 +2166,8 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="10">
+    <row r="14" customHeight="1" spans="1:5">
+      <c r="A14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="11">
@@ -1528,8 +2179,8 @@
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="10">
+    <row r="15" customHeight="1" spans="1:5">
+      <c r="A15" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="11">
@@ -1541,35 +2192,46 @@
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" t="s" s="10">
+    <row r="16" customHeight="1" spans="1:5">
+      <c r="A16" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="11">
         <v>42717.8125</v>
       </c>
       <c r="C16" s="11">
-        <v>42717.972222222219</v>
+        <v>42717.9722222222</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="13"/>
     </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="14">
+    <row r="17" customHeight="1" spans="1:5">
+      <c r="A17" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="15">
         <v>42717.8125</v>
       </c>
       <c r="C17" s="15">
-        <v>42717.972222222219</v>
+        <v>42717.9722222222</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="17"/>
     </row>
+    <row r="18" customHeight="1" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="18">
+        <v>42718.9673611111</v>
+      </c>
+      <c r="C18" s="18">
+        <v>42719.3888888889</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.979167" bottom="0.979167" header="0.509028" footer="0.509028"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="0.979166666666667" bottom="0.979166666666667" header="0.509027777777778" footer="0.509027777777778"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1577,94 +2239,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="18" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="18" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="18" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="18" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="18" customWidth="1"/>
+    <col min="1" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509028" footer="0.509028"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1672,94 +2332,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.17142857142857" defaultRowHeight="12.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.17188" style="19" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="19" customWidth="1"/>
-    <col min="3" max="3" width="9.17188" style="19" customWidth="1"/>
-    <col min="4" max="4" width="9.17188" style="19" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="19" customWidth="1"/>
-    <col min="6" max="256" width="9.17188" style="19" customWidth="1"/>
+    <col min="1" max="256" width="9.17142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509028" footer="0.509028"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>